<commit_message>
reporte y modificacion datos
</commit_message>
<xml_diff>
--- a/InfluenciaDatos.xlsx
+++ b/InfluenciaDatos.xlsx
@@ -2769,7 +2769,7 @@
         <v>3</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="J37" s="8" t="s">
         <v>204</v>
@@ -2874,7 +2874,7 @@
         <v>4</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="J40" s="5" t="s">
         <v>219</v>
@@ -2944,7 +2944,7 @@
         <v>2</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="J42" s="5" t="s">
         <v>229</v>
@@ -2979,7 +2979,7 @@
         <v>3</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="J43" s="8" t="s">
         <v>234</v>

</xml_diff>